<commit_message>
debugged dockerfile, added data
</commit_message>
<xml_diff>
--- a/data/blocks.xlsx
+++ b/data/blocks.xlsx
@@ -1004,7 +1004,7 @@
   </sheetPr>
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C47" activeCellId="0" sqref="C47"/>
     </sheetView>
   </sheetViews>
@@ -2254,7 +2254,7 @@
   </sheetPr>
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
     </sheetView>
   </sheetViews>

</xml_diff>